<commit_message>
figures planned and some draft plots generated; lots of replotting
</commit_message>
<xml_diff>
--- a/05_LookIntoSpecificProteins/out/potential_sulfo_peptidoforms_annotated.xlsx
+++ b/05_LookIntoSpecificProteins/out/potential_sulfo_peptidoforms_annotated.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtzve\Genomics Dropbox\Jordan Tzvetkov\0_Projects\Sulfotyrosine Project\backup_2024_02_15\04_potential_sulfo_peptidoforms_manual_ann\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jtzve\Desktop\Sufo_Tyrosine\05_LookIntoSpecificProteins\out\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{491F6186-3390-4494-858A-EBCB1F9817B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4F4901D-B4FF-49F1-90AE-BFC476FE548F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="potential_sulfo_peptidoforms_an" sheetId="1" r:id="rId1"/>
-    <sheet name="columns_key" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="3" r:id="rId2"/>
+    <sheet name="columns_key" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">potential_sulfo_peptidoforms_an!$A$1:$X$94</definedName>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1921" uniqueCount="966">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1948" uniqueCount="966">
   <si>
     <t>cleaned_protein_IDs</t>
   </si>
@@ -3469,9 +3470,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -3509,7 +3510,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -3615,7 +3616,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -3757,7 +3758,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -3767,8 +3768,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:X94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:X1"/>
+    <sheetView topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9880,10 +9881,160 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11DE0341-0647-4D5E-894F-F579577980CB}">
+  <dimension ref="A1:A27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="R20" sqref="R20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>624</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>75</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79FD9FE3-4F90-49AA-B817-283A40A3E632}">
   <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>

</xml_diff>